<commit_message>
Updated with initiail rxn rates
</commit_message>
<xml_diff>
--- a/Foil_Activation/FoilInfo.xlsx
+++ b/Foil_Activation/FoilInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickq\Documents\AFIT_Masters\NENG612\Foil_Activation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EC0C7D52-9363-4407-B6DD-1D43F9E3014E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A669B5B-4C8F-44D2-A262-058501BA880F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{A54BA526-0B45-47AA-953D-39C722521EAC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{A54BA526-0B45-47AA-953D-39C722521EAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Foil</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Const [s^-1]</t>
   </si>
   <si>
-    <t>Does not include covered Au</t>
-  </si>
-  <si>
     <t>4 Half Lives Brings it up to ~94% of Saturation Activity</t>
   </si>
   <si>
@@ -152,6 +149,87 @@
   </si>
   <si>
     <t xml:space="preserve">The reactions with less than 2 days to reach close to saturation are fine. STAYSL can account for this. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rxn Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">With </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cd Cover </t>
+  </si>
+  <si>
+    <t>CoveredAu-197 (n,2n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoveredAu-197 (n,g) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">without </t>
+  </si>
+  <si>
+    <t>Cover</t>
+  </si>
+  <si>
+    <t>Rel Err</t>
+  </si>
+  <si>
+    <t>Not in staysl or IRDFF</t>
+  </si>
+  <si>
+    <t>Al-27 (n,p)</t>
+  </si>
+  <si>
+    <t>Foil at bottom (Covered Au) Does not seem to be worth adding. The flux is not very thermal. And there seems to be a good amount of difference with position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au-Covered in Rxn Rate without Cover is Au with Cover removed. </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux is not very thermal, so adding a cadmium layer (Cd Cutoff) Did not change the tally by a lot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inclusion of the Cadmium did not have a large impact on the local neutron population. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes on Irradiation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturation </t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>[Bq]</t>
+  </si>
+  <si>
+    <t>Only In-115(n,g),Au-197(n,g),W-186(n,g) feasible</t>
+  </si>
+  <si>
+    <t>Other Possible ones in IRDFF/STAYSL</t>
+  </si>
+  <si>
+    <t>Mg-24</t>
+  </si>
+  <si>
+    <t>Too low of xs</t>
+  </si>
+  <si>
+    <t>Too high of energy</t>
+  </si>
+  <si>
+    <t>Consider Adding</t>
+  </si>
+  <si>
+    <t>Cobalt</t>
+  </si>
+  <si>
+    <t>Copper</t>
   </si>
 </sst>
 </file>
@@ -187,9 +265,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6476E7-6821-4263-8CAF-FA7A6F5D0B49}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +594,7 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -563,7 +642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -595,7 +674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -617,7 +696,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -639,7 +718,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -661,7 +740,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -682,8 +761,11 @@
       <c r="F7">
         <v>0.63500000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -704,8 +786,17 @@
       <c r="F8">
         <v>0.63500000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -726,6 +817,19 @@
       <c r="F9">
         <f>F8</f>
         <v>0.63500000000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -735,25 +839,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9984F67-CDEB-4327-85B1-77D4D7BEF97B}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -761,13 +875,25 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>30</v>
       </c>
@@ -775,13 +901,31 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -801,8 +945,28 @@
         <f>D4/24</f>
         <v>13.06833333333333</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <f>I4*1.006*10^6</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>J4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -811,19 +975,39 @@
         <v>128160</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C13" si="0">LN(2)/B5</f>
+        <f t="shared" ref="C5:C14" si="0">LN(2)/B5</f>
         <v>5.4084517833953281E-6</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D13" si="1">4*B5/(3600)</f>
+        <f t="shared" ref="D5:D14" si="1">4*B5/(3600)</f>
         <v>142.4</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E13" si="2">D5/24</f>
+        <f t="shared" ref="E5:E14" si="2">D5/24</f>
         <v>5.9333333333333336</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" ref="K5:K16" si="3">I5*1.006*10^6</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L14" si="4">J5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -843,8 +1027,28 @@
         <f t="shared" si="2"/>
         <v>309.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G6" s="2">
+        <v>4.5016500000000003E-6</v>
+      </c>
+      <c r="H6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4.5176200000000003E-6</v>
+      </c>
+      <c r="J6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="3"/>
+        <v>4.5447257199999997</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -864,8 +1068,12 @@
         <f t="shared" si="2"/>
         <v>1086.9600000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -885,8 +1093,28 @@
         <f t="shared" si="2"/>
         <v>0.15080555555555555</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G8" s="2">
+        <v>4.2724900000000003E-3</v>
+      </c>
+      <c r="H8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4.3068100000000003E-3</v>
+      </c>
+      <c r="J8">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>4332.6508600000006</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -906,8 +1134,28 @@
         <f t="shared" si="2"/>
         <v>0.74766666666666659</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G9" s="2">
+        <v>3.88822E-6</v>
+      </c>
+      <c r="H9">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3.9041399999999999E-6</v>
+      </c>
+      <c r="J9">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9275648399999996</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -927,8 +1175,28 @@
         <f t="shared" si="2"/>
         <v>24.667600000000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G10" s="2">
+        <v>1.97787E-7</v>
+      </c>
+      <c r="H10">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.9780000000000001E-7</v>
+      </c>
+      <c r="J10">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.19898680000000002</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>4.2599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -948,72 +1216,246 @@
         <f t="shared" si="2"/>
         <v>10.776400000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G11" s="2">
+        <v>4.3278400000000003E-3</v>
+      </c>
+      <c r="H11">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4.3823600000000001E-3</v>
+      </c>
+      <c r="J11">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>4408.65416</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>8.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="G12" s="2">
+        <v>2.2802500000000001E-7</v>
+      </c>
+      <c r="H12">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2.28206E-7</v>
+      </c>
+      <c r="J12">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22957523599999999</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="4"/>
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <f>14.997*60*60</f>
         <v>53989.2</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>1.2838626624583163E-5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>59.988</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <f t="shared" si="2"/>
         <v>2.4994999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="G13" s="2">
+        <v>6.0026100000000003E-8</v>
+      </c>
+      <c r="H13">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.0001799999999999E-8</v>
+      </c>
+      <c r="J13">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>6.0361810799999992E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>8.0225368120364038E-6</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G14" s="2">
+        <v>5.4107600000000004E-4</v>
+      </c>
+      <c r="H14">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5.4651199999999997E-4</v>
+      </c>
+      <c r="J14">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>549.79107199999987</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="4"/>
+        <v>1.0699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <f>6.1669*60*60*24</f>
+        <v>532820.16</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:C16" si="5">LN(2)/B15</f>
+        <v>1.3009026921202555E-6</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" ref="D15:D16" si="6">4*B15/(3600)</f>
+        <v>592.02240000000006</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E16" si="7">D15/24</f>
+        <v>24.667600000000004</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.00845E-7</v>
+      </c>
+      <c r="H15">
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.9999000000000001E-7</v>
+      </c>
+      <c r="J15">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <f>2.6941*24*60*60</f>
+        <v>232770.24</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="5"/>
+        <v>2.9778170120026741E-6</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="6"/>
+        <v>258.6336</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>10.776400000000001</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4.4166700000000001E-3</v>
+      </c>
+      <c r="H16">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I16" s="2">
+        <v>4.4940500000000003E-3</v>
+      </c>
+      <c r="J16">
+        <v>7.6E-3</v>
+      </c>
+      <c r="K16" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>